<commit_message>
Alterações  func Wood + implemento func cooking
</commit_message>
<xml_diff>
--- a/cooking.xlsx
+++ b/cooking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gardingo/Documents/Python/Projeto Melvor Calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7C52CA6-FA01-EE46-A739-8C954B381242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E66C92-C18F-DA46-A4C4-14784D3472A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1900" windowWidth="28040" windowHeight="17360" xr2:uid="{D0F46FF9-9BEB-5F46-AA86-654E48B49B50}"/>
+    <workbookView xWindow="9200" yWindow="2840" windowWidth="11320" windowHeight="17360" xr2:uid="{D0F46FF9-9BEB-5F46-AA86-654E48B49B50}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Xp</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Whale</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -446,151 +449,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85C77FD-CC19-1645-831F-43ABC491CF62}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="1">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="1">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" s="1">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" s="1">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="1">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1">
         <v>150</v>
       </c>
+      <c r="C17" s="1">
+        <v>2048</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
0.0.4 layout cooking modificado
</commit_message>
<xml_diff>
--- a/cooking.xlsx
+++ b/cooking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gardingo/Documents/Python/Projeto Melvor Calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E66C92-C18F-DA46-A4C4-14784D3472A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D458A9-0C7C-374A-A855-744C23161DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9200" yWindow="2840" windowWidth="11320" windowHeight="17360" xr2:uid="{D0F46FF9-9BEB-5F46-AA86-654E48B49B50}"/>
+    <workbookView xWindow="24320" yWindow="3800" windowWidth="11320" windowHeight="17360" xr2:uid="{D0F46FF9-9BEB-5F46-AA86-654E48B49B50}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Xp</t>
   </si>
   <si>
-    <t>Fish</t>
-  </si>
-  <si>
     <t>Shrimp</t>
   </si>
   <si>
@@ -90,6 +87,45 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Oak</t>
+  </si>
+  <si>
+    <t>Willow</t>
+  </si>
+  <si>
+    <t>Teak</t>
+  </si>
+  <si>
+    <t>Maple</t>
+  </si>
+  <si>
+    <t>Mahogany</t>
+  </si>
+  <si>
+    <t>Yew</t>
+  </si>
+  <si>
+    <t>Magic</t>
+  </si>
+  <si>
+    <t>Redwood</t>
+  </si>
+  <si>
+    <t>Logs</t>
+  </si>
+  <si>
+    <t>Bonus Xp</t>
+  </si>
+  <si>
+    <t>Beef</t>
+  </si>
+  <si>
+    <t>Recipe Cooking Fire</t>
   </si>
 </sst>
 </file>
@@ -132,9 +168,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,28 +488,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85C77FD-CC19-1645-831F-43ABC491CF62}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>5</v>
@@ -478,169 +526,234 @@
       <c r="C2" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B5" s="1">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1">
         <v>10</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1">
+        <v>65</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="B7" s="1">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2">
         <v>30</v>
       </c>
-      <c r="C5" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B8" s="1">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1">
+        <v>58</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>40</v>
+      </c>
+      <c r="C9" s="1">
+        <v>108</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>30</v>
-      </c>
-      <c r="C7" s="1">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="E9" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
-        <v>40</v>
-      </c>
-      <c r="C8" s="1">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="B10" s="1">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1">
+        <v>134</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" s="1">
-        <v>50</v>
-      </c>
-      <c r="C9" s="1">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1">
-        <v>60</v>
-      </c>
-      <c r="C10" s="1">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="B11" s="1">
         <v>60</v>
       </c>
       <c r="C11" s="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>60</v>
+      </c>
+      <c r="C12" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>70</v>
+      </c>
+      <c r="C13" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1">
-        <v>70</v>
-      </c>
-      <c r="C12" s="1">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="B14" s="1">
+        <v>75</v>
+      </c>
+      <c r="C14" s="1">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1">
-        <v>75</v>
-      </c>
-      <c r="C13" s="1">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="B15" s="1">
+        <v>80</v>
+      </c>
+      <c r="C15" s="1">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1">
-        <v>80</v>
-      </c>
-      <c r="C14" s="1">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <v>100</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C16" s="1">
         <v>538</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="1">
-        <v>125</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1624</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
+        <v>125</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
         <v>150</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C18" s="1">
         <v>2048</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0.0.6 corrigindo skill xp/hr - cooking
</commit_message>
<xml_diff>
--- a/cooking.xlsx
+++ b/cooking.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gardingo/Documents/Python/Projeto Melvor Calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D458A9-0C7C-374A-A855-744C23161DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5259E64-D14B-B147-A611-34C48736CC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24320" yWindow="3800" windowWidth="11320" windowHeight="17360" xr2:uid="{D0F46FF9-9BEB-5F46-AA86-654E48B49B50}"/>
+    <workbookView xWindow="11720" yWindow="2180" windowWidth="15160" windowHeight="17360" xr2:uid="{D0F46FF9-9BEB-5F46-AA86-654E48B49B50}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Xp</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Recipe Cooking Fire</t>
+  </si>
+  <si>
+    <t>Cook Time</t>
   </si>
 </sst>
 </file>
@@ -488,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85C77FD-CC19-1645-831F-43ABC491CF62}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="G1" sqref="G1:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,7 +502,7 @@
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -510,13 +513,17 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -526,14 +533,17 @@
       <c r="C2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -543,14 +553,17 @@
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -560,14 +573,17 @@
       <c r="C4" s="1">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -577,14 +593,17 @@
       <c r="C5" s="1">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -594,14 +613,17 @@
       <c r="C6" s="1">
         <v>65</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -611,14 +633,17 @@
       <c r="C7" s="1">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -628,14 +653,17 @@
       <c r="C8" s="1">
         <v>58</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -645,14 +673,17 @@
       <c r="C9" s="1">
         <v>108</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -662,14 +693,17 @@
       <c r="C10" s="1">
         <v>134</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -679,8 +713,11 @@
       <c r="C11" s="1">
         <v>209</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -690,8 +727,11 @@
       <c r="C12" s="1">
         <v>250</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -701,8 +741,11 @@
       <c r="C13" s="1">
         <v>280</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -712,8 +755,11 @@
       <c r="C14" s="1">
         <v>395</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -723,8 +769,11 @@
       <c r="C15" s="1">
         <v>674</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -734,8 +783,11 @@
       <c r="C16" s="1">
         <v>538</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -745,8 +797,11 @@
       <c r="C17" s="1">
         <v>1624</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -755,6 +810,9 @@
       </c>
       <c r="C18" s="1">
         <v>2048</v>
+      </c>
+      <c r="D18">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.0.7 terminando a logica do Cooking
</commit_message>
<xml_diff>
--- a/cooking.xlsx
+++ b/cooking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gardingo/Documents/Python/Projeto Melvor Calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5259E64-D14B-B147-A611-34C48736CC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B0BBB5-B33D-0244-8374-45E3B4E972A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11720" yWindow="2180" windowWidth="15160" windowHeight="17360" xr2:uid="{D0F46FF9-9BEB-5F46-AA86-654E48B49B50}"/>
+    <workbookView xWindow="23240" yWindow="3920" windowWidth="15160" windowHeight="17360" xr2:uid="{D0F46FF9-9BEB-5F46-AA86-654E48B49B50}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Xp</t>
   </si>
@@ -129,6 +129,48 @@
   </si>
   <si>
     <t>Cook Time</t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Plain Pizza Slice</t>
+  </si>
+  <si>
+    <t>Beef Pie</t>
+  </si>
+  <si>
+    <t>Meat Pizza Slice</t>
+  </si>
+  <si>
+    <t>Strawberry Cupcake</t>
+  </si>
+  <si>
+    <t>Cherry Cupcake</t>
+  </si>
+  <si>
+    <t>Apple Pie</t>
+  </si>
+  <si>
+    <t>Strawberry Cake</t>
+  </si>
+  <si>
+    <t>Carrot Cake</t>
+  </si>
+  <si>
+    <t>Basic Soup</t>
+  </si>
+  <si>
+    <t>Hearty Soup</t>
+  </si>
+  <si>
+    <t>Cream Corn Soup</t>
+  </si>
+  <si>
+    <t>Chicken Soup</t>
   </si>
 </sst>
 </file>
@@ -491,15 +533,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85C77FD-CC19-1645-831F-43ABC491CF62}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G18"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -585,16 +627,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>21</v>
@@ -605,16 +647,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>22</v>
@@ -625,13 +667,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -645,13 +687,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -665,13 +707,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -685,16 +727,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>26</v>
@@ -705,114 +747,310 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1">
-        <v>250</v>
+        <v>134</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C13" s="1">
-        <v>280</v>
+        <v>209</v>
       </c>
       <c r="D13">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C14" s="1">
-        <v>395</v>
+        <v>250</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C15" s="1">
-        <v>674</v>
+        <v>280</v>
       </c>
       <c r="D15">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B16" s="1">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="C16" s="1">
-        <v>538</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="C17" s="1">
-        <v>1624</v>
+        <v>395</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>80</v>
+      </c>
+      <c r="C18" s="1">
+        <v>674</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>100</v>
+      </c>
+      <c r="C19" s="1">
+        <v>538</v>
+      </c>
+      <c r="D19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="1">
+        <v>161</v>
+      </c>
+      <c r="C20" s="1">
+        <v>37</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1">
+        <v>125</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1624</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1">
+        <v>126</v>
+      </c>
+      <c r="C22" s="1">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B23" s="1">
         <v>150</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C23" s="1">
         <v>2048</v>
       </c>
-      <c r="D18">
+      <c r="D23">
         <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="1">
+        <v>161</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="1">
+        <v>214</v>
+      </c>
+      <c r="C25" s="1">
+        <v>42</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="1">
+        <v>223</v>
+      </c>
+      <c r="C26" s="1">
+        <v>22</v>
+      </c>
+      <c r="D26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1">
+        <v>252</v>
+      </c>
+      <c r="C27" s="1">
+        <v>78</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="1">
+        <v>274</v>
+      </c>
+      <c r="C28" s="1">
+        <v>42</v>
+      </c>
+      <c r="D28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="1">
+        <v>424</v>
+      </c>
+      <c r="C29" s="1">
+        <v>253</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="1">
+        <v>490</v>
+      </c>
+      <c r="C30" s="1">
+        <v>378</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="1">
+        <v>603</v>
+      </c>
+      <c r="C31" s="1">
+        <v>751</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="1">
+        <v>617</v>
+      </c>
+      <c r="C32" s="1">
+        <v>96</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>